<commit_message>
Medição da Sprint 7 realizada
</commit_message>
<xml_diff>
--- a/docs/project/STE_MED_Registro de Medição.xlsx
+++ b/docs/project/STE_MED_Registro de Medição.xlsx
@@ -432,7 +432,7 @@
               <a:gsLst>
                 <a:gs pos="0">
                   <a:schemeClr val="accent1">
-                    <a:tint val="77000"/>
+                    <a:tint val="65000"/>
                     <a:satMod val="103000"/>
                     <a:lumMod val="102000"/>
                     <a:tint val="94000"/>
@@ -440,7 +440,7 @@
                 </a:gs>
                 <a:gs pos="50000">
                   <a:schemeClr val="accent1">
-                    <a:tint val="77000"/>
+                    <a:tint val="65000"/>
                     <a:satMod val="110000"/>
                     <a:lumMod val="100000"/>
                     <a:shade val="100000"/>
@@ -448,7 +448,7 @@
                 </a:gs>
                 <a:gs pos="100000">
                   <a:schemeClr val="accent1">
-                    <a:tint val="77000"/>
+                    <a:tint val="65000"/>
                     <a:lumMod val="99000"/>
                     <a:satMod val="120000"/>
                     <a:shade val="78000"/>
@@ -590,7 +590,6 @@
               <a:gsLst>
                 <a:gs pos="0">
                   <a:schemeClr val="accent1">
-                    <a:shade val="76000"/>
                     <a:satMod val="103000"/>
                     <a:lumMod val="102000"/>
                     <a:tint val="94000"/>
@@ -598,7 +597,6 @@
                 </a:gs>
                 <a:gs pos="50000">
                   <a:schemeClr val="accent1">
-                    <a:shade val="76000"/>
                     <a:satMod val="110000"/>
                     <a:lumMod val="100000"/>
                     <a:shade val="100000"/>
@@ -606,7 +604,6 @@
                 </a:gs>
                 <a:gs pos="100000">
                   <a:schemeClr val="accent1">
-                    <a:shade val="76000"/>
                     <a:lumMod val="99000"/>
                     <a:satMod val="120000"/>
                     <a:shade val="78000"/>
@@ -726,6 +723,166 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1117-4524-8B51-E5F341547BE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Registro!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="65000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="65000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="65000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Registro!$C$7:$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>GERÊNCIA DE REQUISITOS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GERÊNCIA DE PROJETOS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GERÊNCIA DE CONFIGURAÇÃO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GERÊNCIA DE QUALIDADE</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MEDIÇÃO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Registro!$C$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE53-4379-A7BD-5703FDC7104E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -933,7 +1090,11 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="97000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -979,8 +1140,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.43888955713673278"/>
           <c:y val="0.92907293630549703"/>
-          <c:w val="0.12065410155105465"/>
-          <c:h val="6.6176933765632232E-2"/>
+          <c:w val="7.9249493813273342E-2"/>
+          <c:h val="6.3380725296661874E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1933,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,12 +2441,24 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="7">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>116</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3358,13 +3531,13 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B16">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B16">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:G9 C8:C16">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:G10 C8:C16">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 B8">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B10">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>